<commit_message>
file organization and working copy and paste svalues only; handling multi-pcps and order files
</commit_message>
<xml_diff>
--- a/files/9ZEB_Order 2_FaceTalk_Uzbek.xlsx
+++ b/files/9ZEB_Order 2_FaceTalk_Uzbek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shakhlonematova/Library/Mobile Documents/com~apple~CloudDocs/PhD/Projects/QP2_FaceTalk/Data Analysis/Uzbek/9ZEB_Order 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharjianto/Documents/Projects/order-analysis/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA343DA-B228-914A-BC57-1187BEB5B12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE1136C-E648-0D45-8025-1A352E5943EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16960" yWindow="1160" windowWidth="10660" windowHeight="16240" xr2:uid="{52EE2B89-7F22-E148-AEE2-0D6F718BCAB1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{52EE2B89-7F22-E148-AEE2-0D6F718BCAB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -647,6 +647,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -669,12 +675,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C141924-F4C7-F84B-8322-57E90498B8EB}">
   <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,18 +1075,18 @@
       <c r="T1" s="9"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="13"/>
@@ -2912,18 +2912,18 @@
       <c r="K41" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L41" s="37" t="s">
+      <c r="L41" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="M41" s="37"/>
-      <c r="N41" s="37"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
       <c r="P41" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q41" s="37" t="s">
+      <c r="Q41" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="R41" s="37"/>
+      <c r="R41" s="30"/>
     </row>
     <row r="42" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -2950,20 +2950,20 @@
       <c r="K42" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L42" s="38">
+      <c r="L42" s="29">
         <f>Q26-Q10</f>
         <v>-0.59360730593607303</v>
       </c>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
       <c r="P42" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="Q42" s="38">
+      <c r="Q42" s="29">
         <f t="shared" ref="Q42:Q47" si="3">Q34-Q18</f>
         <v>0.26809511366605698</v>
       </c>
-      <c r="R42" s="38"/>
+      <c r="R42" s="29"/>
     </row>
     <row r="43" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -2993,20 +2993,20 @@
       <c r="K43" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="L43" s="38">
+      <c r="L43" s="29">
         <f>Q27-Q11</f>
         <v>7.5545410649225153E-2</v>
       </c>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
       <c r="P43" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="Q43" s="38">
+      <c r="Q43" s="29">
         <f t="shared" si="3"/>
         <v>8.4085727314181513E-2</v>
       </c>
-      <c r="R43" s="38"/>
+      <c r="R43" s="29"/>
     </row>
     <row r="44" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -3036,20 +3036,20 @@
       <c r="K44" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="L44" s="38">
+      <c r="L44" s="29">
         <f>Q28-Q12</f>
         <v>-0.23809935952916733</v>
       </c>
-      <c r="M44" s="38"/>
-      <c r="N44" s="38"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
       <c r="P44" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Q44" s="38">
+      <c r="Q44" s="29">
         <f>Q36-Q20</f>
         <v>-0.31532575933225127</v>
       </c>
-      <c r="R44" s="38"/>
+      <c r="R44" s="29"/>
     </row>
     <row r="45" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
@@ -3076,20 +3076,20 @@
       <c r="K45" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="L45" s="38">
+      <c r="L45" s="29">
         <f>Q29-Q13</f>
         <v>5.7609057609057657E-2</v>
       </c>
-      <c r="M45" s="38"/>
-      <c r="N45" s="38"/>
+      <c r="M45" s="29"/>
+      <c r="N45" s="29"/>
       <c r="P45" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="Q45" s="38">
+      <c r="Q45" s="29">
         <f t="shared" si="3"/>
         <v>-0.23269980506822607</v>
       </c>
-      <c r="R45" s="38"/>
+      <c r="R45" s="29"/>
     </row>
     <row r="46" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
@@ -3119,20 +3119,20 @@
       <c r="K46" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="L46" s="38">
+      <c r="L46" s="29">
         <f>Q30-Q14</f>
         <v>0.65432098765432101</v>
       </c>
-      <c r="M46" s="38"/>
-      <c r="N46" s="38"/>
+      <c r="M46" s="29"/>
+      <c r="N46" s="29"/>
       <c r="P46" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="Q46" s="38">
+      <c r="Q46" s="29">
         <f t="shared" si="3"/>
         <v>-3.0051256613756627E-2</v>
       </c>
-      <c r="R46" s="38"/>
+      <c r="R46" s="29"/>
     </row>
     <row r="47" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
@@ -3162,20 +3162,20 @@
       <c r="K47" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="L47" s="38">
+      <c r="L47" s="29">
         <f t="shared" ref="L47" si="4">Q31-Q15</f>
         <v>0.17237265464010698</v>
       </c>
-      <c r="M47" s="38"/>
-      <c r="N47" s="38"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
       <c r="P47" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Q47" s="38">
+      <c r="Q47" s="29">
         <f t="shared" si="3"/>
         <v>0.57555178268251272</v>
       </c>
-      <c r="R47" s="38"/>
+      <c r="R47" s="29"/>
     </row>
     <row r="48" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -3267,19 +3267,19 @@
       <c r="H50" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J50" s="34" t="s">
+      <c r="J50" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="36"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="38"/>
       <c r="P50" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q50" s="37" t="s">
+      <c r="Q50" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="R50" s="37"/>
+      <c r="R50" s="30"/>
     </row>
     <row r="51" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
@@ -3303,7 +3303,7 @@
       <c r="H51" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J51" s="30" t="s">
+      <c r="J51" s="32" t="s">
         <v>34</v>
       </c>
       <c r="K51" s="10" t="s">
@@ -3321,11 +3321,11 @@
       <c r="P51" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="Q51" s="38">
+      <c r="Q51" s="29">
         <f>Q34-Q26</f>
         <v>0.95348837209302328</v>
       </c>
-      <c r="R51" s="38"/>
+      <c r="R51" s="29"/>
     </row>
     <row r="52" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
@@ -3352,7 +3352,7 @@
       <c r="H52" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="J52" s="30"/>
+      <c r="J52" s="32"/>
       <c r="K52" s="11" t="s">
         <v>60</v>
       </c>
@@ -3370,11 +3370,11 @@
       <c r="P52" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="Q52" s="38">
+      <c r="Q52" s="29">
         <f t="shared" ref="Q52:Q56" si="5">Q35-Q27</f>
         <v>0.37839100923556257</v>
       </c>
-      <c r="R52" s="38"/>
+      <c r="R52" s="29"/>
     </row>
     <row r="53" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -3401,7 +3401,7 @@
       <c r="H53" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J53" s="30"/>
+      <c r="J53" s="32"/>
       <c r="K53" s="11" t="s">
         <v>114</v>
       </c>
@@ -3420,11 +3420,11 @@
       <c r="P53" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Q53" s="38">
+      <c r="Q53" s="29">
         <f>Q36-Q28</f>
         <v>0.16610333172380493</v>
       </c>
-      <c r="R53" s="38"/>
+      <c r="R53" s="29"/>
     </row>
     <row r="54" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -3448,7 +3448,7 @@
       <c r="H54" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J54" s="30"/>
+      <c r="J54" s="32"/>
       <c r="K54" s="11" t="s">
         <v>88</v>
       </c>
@@ -3466,11 +3466,11 @@
       <c r="P54" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="Q54" s="38">
+      <c r="Q54" s="29">
         <f t="shared" si="5"/>
         <v>0.19883357383357386</v>
       </c>
-      <c r="R54" s="38"/>
+      <c r="R54" s="29"/>
     </row>
     <row r="55" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -3497,7 +3497,7 @@
       <c r="H55" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="J55" s="30"/>
+      <c r="J55" s="32"/>
       <c r="K55" s="11" t="s">
         <v>71</v>
       </c>
@@ -3516,11 +3516,11 @@
       <c r="P55" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="Q55" s="38">
+      <c r="Q55" s="29">
         <f t="shared" si="5"/>
         <v>7.2241512345678993E-2</v>
       </c>
-      <c r="R55" s="38"/>
+      <c r="R55" s="29"/>
     </row>
     <row r="56" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
@@ -3547,7 +3547,7 @@
       <c r="H56" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J56" s="30"/>
+      <c r="J56" s="32"/>
       <c r="K56" s="11" t="s">
         <v>61</v>
       </c>
@@ -3562,11 +3562,11 @@
       <c r="P56" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Q56" s="38">
+      <c r="Q56" s="29">
         <f t="shared" si="5"/>
         <v>0.13367370619633334</v>
       </c>
-      <c r="R56" s="38"/>
+      <c r="R56" s="29"/>
     </row>
     <row r="57" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
@@ -3590,7 +3590,7 @@
       <c r="H57" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J57" s="31"/>
+      <c r="J57" s="33"/>
       <c r="K57" s="11" t="s">
         <v>100</v>
       </c>
@@ -3633,7 +3633,7 @@
       <c r="H58" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="J58" s="32" t="s">
+      <c r="J58" s="34" t="s">
         <v>37</v>
       </c>
       <c r="K58" s="11" t="s">
@@ -3650,10 +3650,10 @@
       <c r="P58" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Q58" s="37" t="s">
+      <c r="Q58" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="R58" s="37"/>
+      <c r="R58" s="30"/>
     </row>
     <row r="59" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -3680,7 +3680,7 @@
       <c r="H59" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J59" s="32"/>
+      <c r="J59" s="34"/>
       <c r="K59" s="11" t="s">
         <v>114</v>
       </c>
@@ -3698,11 +3698,11 @@
       <c r="P59" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="Q59" s="38">
+      <c r="Q59" s="29">
         <f t="shared" ref="Q59:Q63" si="6">Q18-Q10</f>
         <v>9.1785952490893274E-2</v>
       </c>
-      <c r="R59" s="38"/>
+      <c r="R59" s="29"/>
     </row>
     <row r="60" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
@@ -3726,7 +3726,7 @@
       <c r="H60" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J60" s="32"/>
+      <c r="J60" s="34"/>
       <c r="K60" s="11" t="s">
         <v>88</v>
       </c>
@@ -3745,11 +3745,11 @@
       <c r="P60" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="Q60" s="38">
+      <c r="Q60" s="29">
         <f t="shared" si="6"/>
         <v>0.36985069257060621</v>
       </c>
-      <c r="R60" s="38"/>
+      <c r="R60" s="29"/>
     </row>
     <row r="61" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
@@ -3776,7 +3776,7 @@
       <c r="H61" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="J61" s="32"/>
+      <c r="J61" s="34"/>
       <c r="K61" s="11" t="s">
         <v>71</v>
       </c>
@@ -3794,11 +3794,11 @@
       <c r="P61" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Q61" s="38">
+      <c r="Q61" s="29">
         <f t="shared" si="6"/>
         <v>0.24332973152688886</v>
       </c>
-      <c r="R61" s="38"/>
+      <c r="R61" s="29"/>
     </row>
     <row r="62" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -3825,7 +3825,7 @@
       <c r="H62" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="J62" s="32"/>
+      <c r="J62" s="34"/>
       <c r="K62" s="11" t="s">
         <v>61</v>
       </c>
@@ -3844,11 +3844,11 @@
       <c r="P62" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="Q62" s="38">
+      <c r="Q62" s="29">
         <f>Q21-Q13</f>
         <v>0.48914243651085759</v>
       </c>
-      <c r="R62" s="38"/>
+      <c r="R62" s="29"/>
     </row>
     <row r="63" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
@@ -3872,7 +3872,7 @@
       <c r="H63" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="J63" s="33"/>
+      <c r="J63" s="35"/>
       <c r="K63" s="11" t="s">
         <v>100</v>
       </c>
@@ -3887,11 +3887,11 @@
       <c r="P63" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="Q63" s="38">
+      <c r="Q63" s="29">
         <f t="shared" si="6"/>
         <v>0.75661375661375663</v>
       </c>
-      <c r="R63" s="38"/>
+      <c r="R63" s="29"/>
     </row>
     <row r="64" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
@@ -3922,11 +3922,11 @@
       <c r="P64" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Q64" s="38">
+      <c r="Q64" s="29">
         <f>Q23-Q15</f>
         <v>-0.26950542184607246</v>
       </c>
-      <c r="R64" s="38"/>
+      <c r="R64" s="29"/>
     </row>
     <row r="65" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
@@ -4312,13 +4312,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="Q63:R63"/>
-    <mergeCell ref="Q64:R64"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="Q59:R59"/>
-    <mergeCell ref="Q60:R60"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="J51:J57"/>
+    <mergeCell ref="J58:J63"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="Q44:R44"/>
     <mergeCell ref="Q45:R45"/>
     <mergeCell ref="Q46:R46"/>
     <mergeCell ref="Q55:R55"/>
@@ -4332,18 +4337,13 @@
     <mergeCell ref="Q52:R52"/>
     <mergeCell ref="Q53:R53"/>
     <mergeCell ref="Q54:R54"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="J51:J57"/>
-    <mergeCell ref="J58:J63"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="Q64:R64"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="Q59:R59"/>
+    <mergeCell ref="Q60:R60"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="Q62:R62"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">

</xml_diff>